<commit_message>
Se agrega datos de Arequipa desde el 01-01-23 hasta el 31-08-23
</commit_message>
<xml_diff>
--- a/DATOS_VENTA_23.xlsx
+++ b/DATOS_VENTA_23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENTOS\ESPECIALIZACION DATA ANALYTICS\dataops\trabajo_final_dataops2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DAFD3E-94EC-47F0-B2F4-697D63B8608A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12211E1-5583-41C4-9BC5-FB78C0DCDDF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{298EFFE4-52CD-4160-8C02-56F0080C6DFB}"/>
   </bookViews>
@@ -550,7 +550,7 @@
   <dimension ref="A1:E427"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>